<commit_message>
Create the results table
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -69,7 +72,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
LocalT2 check repeated coverage
There is no repeated coverage
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -72,7 +75,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
StanDep with Lucia Code
I run it but is not important, the important part is that I have lucia's code
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -75,7 +81,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Create a live script for LocalT2 and localgini
Just create a livescript for both of them. I still have to comment them and clean the github
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -99,7 +102,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
LocalT2 solved and Enzymes thing
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -132,247 +141,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>72.612612612612608</v>
+        <v>73.693693693693689</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>71.531531531531527</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>73.513513513513516</v>
+        <v>75.675675675675677</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>68.468468468468473</v>
+        <v>69.729729729729726</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>70.990990990990994</v>
+        <v>72.612612612612608</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>70.810810810810807</v>
+        <v>72.612612612612608</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>78.918918918918919</v>
+        <v>80.540540540540533</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>79.099099099099107</v>
+        <v>81.081081081081081</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>78.198198198198199</v>
+        <v>79.459459459459453</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>79.63963963963964</v>
+        <v>80.36036036036036</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>66.666666666666657</v>
+        <v>67.567567567567565</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>70.450450450450447</v>
+        <v>72.612612612612608</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>75.855855855855864</v>
+        <v>76.396396396396398</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>75.13513513513513</v>
+        <v>76.396396396396398</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>75.13513513513513</v>
+        <v>76.936936936936945</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>63.243243243243242</v>
+        <v>64.684684684684697</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>66.486486486486484</v>
+        <v>67.747747747747738</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>70.090090090090087</v>
+        <v>71.171171171171167</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>76.576576576576571</v>
+        <v>77.837837837837839</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>78.198198198198199</v>
+        <v>79.099099099099107</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>76.936936936936945</v>
+        <v>78.378378378378372</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>65.765765765765778</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>63.063063063063062</v>
+        <v>64.504504504504496</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>62.702702702702709</v>
+        <v>64.324324324324323</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>73.873873873873876</v>
+        <v>75.49549549549549</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>70.270270270270274</v>
+        <v>72.252252252252248</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>70.990990990990994</v>
+        <v>74.054054054054049</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>70.990990990990994</v>
+        <v>72.972972972972968</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>67.747747747747738</v>
+        <v>69.549549549549553</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>70.630630630630634</v>
+        <v>72.972972972972968</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>72.612612612612608</v>
+        <v>75.49549549549549</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>73.693693693693689</v>
+        <v>75.855855855855864</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>73.873873873873876</v>
+        <v>76.396396396396398</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>67.567567567567565</v>
+        <v>69.009009009009006</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>68.108108108108112</v>
+        <v>69.549549549549553</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>61.981981981981981</v>
+        <v>63.063063063063062</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.369369369369366</v>
+        <v>70.990990990990994</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>64.684684684684697</v>
+        <v>66.306306306306311</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>65.765765765765778</v>
+        <v>66.846846846846844</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>71.891891891891888</v>
+        <v>74.414414414414409</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.414414414414409</v>
+        <v>76.396396396396398</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>74.234234234234236</v>
+        <v>76.756756756756758</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.054054054054049</v>
+        <v>75.675675675675677</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>74.054054054054049</v>
+        <v>76.036036036036037</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>74.954954954954957</v>
+        <v>75.675675675675677</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>67.387387387387392</v>
+        <v>68.648648648648646</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>67.747747747747738</v>
+        <v>68.468468468468473</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>71.351351351351354</v>
+        <v>73.693693693693689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in localT2 for different hk lists
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -159,247 +165,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>74.228675136116152</v>
+        <v>84.81481481481481</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>73.865698729582576</v>
+        <v>83.703703703703695</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>76.225045372050815</v>
+        <v>85.18518518518519</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>70.235934664246827</v>
+        <v>79.629629629629633</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>73.139745916515437</v>
+        <v>81.481481481481481</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>73.139745916515437</v>
+        <v>81.481481481481481</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>81.125226860254088</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>81.669691470054445</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>80.036297640653359</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>80.943738656987293</v>
+        <v>88.518518518518519</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>68.058076225045369</v>
+        <v>76.296296296296291</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>73.139745916515437</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76.950998185117967</v>
+        <v>88.518518518518519</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>76.950998185117967</v>
+        <v>87.407407407407405</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>77.495462794918339</v>
+        <v>88.148148148148152</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>65.154264972776758</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>68.239564428312164</v>
+        <v>81.851851851851848</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>71.687840290381118</v>
+        <v>84.074074074074076</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78.402903811252273</v>
+        <v>85.925925925925924</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>79.673321234119783</v>
+        <v>87.407407407407405</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>78.94736842105263</v>
+        <v>87.407407407407405</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>67.150635208711435</v>
+        <v>77.777777777777786</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>64.972776769509977</v>
+        <v>77.407407407407405</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>64.791288566243196</v>
+        <v>76.296296296296291</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>76.043557168784019</v>
+        <v>87.407407407407405</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>72.776769509981847</v>
+        <v>84.444444444444443</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>74.591651542649728</v>
+        <v>85.555555555555557</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>73.502722323048999</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>70.054446460980031</v>
+        <v>81.851851851851848</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>73.502722323048999</v>
+        <v>83.703703703703695</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>76.043557168784019</v>
+        <v>81.851851851851848</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>76.40653357531761</v>
+        <v>82.962962962962962</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>76.950998185117967</v>
+        <v>82.222222222222214</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>69.509981851179674</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.054446460980031</v>
+        <v>80.370370370370367</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>63.520871143375679</v>
+        <v>78.518518518518519</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>71.506352087114337</v>
+        <v>80.370370370370367</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>66.787658802177859</v>
+        <v>77.407407407407405</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>67.332123411978216</v>
+        <v>77.407407407407405</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.954627949183305</v>
+        <v>85.925925925925924</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>76.950998185117967</v>
+        <v>87.037037037037038</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>77.313974591651544</v>
+        <v>86.296296296296291</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>76.225045372050815</v>
+        <v>85.555555555555557</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>76.588021778584391</v>
+        <v>85.925925925925924</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>76.225045372050815</v>
+        <v>85.555555555555557</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>69.147005444646098</v>
+        <v>78.888888888888886</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>68.965517241379317</v>
+        <v>79.629629629629633</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>74.228675136116152</v>
+        <v>84.074074074074076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in StanDep to make it more reproducible
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -165,7 +168,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
change in the housekeeeping accuracy
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -174,7 +183,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Changes to impove the localT2
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -183,247 +192,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>73.139745916515437</v>
+        <v>74.228675136116152</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>72.050816696914694</v>
+        <v>73.865698729582576</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>74.047186932849357</v>
+        <v>76.225045372050815</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>68.965517241379317</v>
+        <v>70.235934664246827</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71.506352087114337</v>
+        <v>73.139745916515437</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71.324863883847542</v>
+        <v>73.139745916515437</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>79.491833030853002</v>
+        <v>80.943738656987293</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>79.673321234119783</v>
+        <v>81.669691470054445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>78.765880217785849</v>
+        <v>80.036297640653359</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>80.21778584392014</v>
+        <v>80.943738656987293</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>67.150635208711435</v>
+        <v>68.058076225045369</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>70.961887477313979</v>
+        <v>72.776769509981847</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76.40653357531761</v>
+        <v>76.769509981851186</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>75.680580762250443</v>
+        <v>76.950998185117967</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>75.680580762250443</v>
+        <v>77.495462794918339</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>63.702359346642467</v>
+        <v>64.791288566243196</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>66.969147005444654</v>
+        <v>68.058076225045369</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>70.598911070780403</v>
+        <v>71.687840290381118</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>77.132486388384763</v>
+        <v>78.402903811252273</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>78.765880217785849</v>
+        <v>79.673321234119783</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>77.495462794918339</v>
+        <v>78.94736842105263</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>66.243194192377501</v>
+        <v>66.969147005444654</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>63.520871143375679</v>
+        <v>64.791288566243196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>63.157894736842103</v>
+        <v>64.609800362976415</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>74.410163339382933</v>
+        <v>76.043557168784019</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>70.780399274047184</v>
+        <v>72.41379310344827</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>71.506352087114337</v>
+        <v>74.591651542649728</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>71.506352087114337</v>
+        <v>73.321234119782218</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>68.239564428312164</v>
+        <v>70.054446460980031</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>71.14337568058076</v>
+        <v>73.502722323048999</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>73.139745916515437</v>
+        <v>75.862068965517238</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>74.228675136116152</v>
+        <v>76.40653357531761</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>74.410163339382933</v>
+        <v>76.588021778584391</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>68.058076225045369</v>
+        <v>69.509981851179674</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>68.60254083484574</v>
+        <v>70.054446460980031</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>62.431941923774957</v>
+        <v>63.339382940108891</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.87295825771325</v>
+        <v>71.506352087114337</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>65.154264972776758</v>
+        <v>66.787658802177859</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>66.243194192377501</v>
+        <v>67.150635208711435</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>72.41379310344827</v>
+        <v>74.954627949183305</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74.954627949183305</v>
+        <v>76.769509981851186</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>74.773139745916524</v>
+        <v>77.313974591651544</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>74.591651542649728</v>
+        <v>76.043557168784019</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>74.591651542649728</v>
+        <v>76.40653357531761</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>75.499092558983676</v>
+        <v>76.225045372050815</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>67.876588021778588</v>
+        <v>68.965517241379317</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>68.239564428312164</v>
+        <v>68.784029038112521</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>71.869328493647913</v>
+        <v>74.047186932849357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved code in compare HKG_Lists
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -213,247 +216,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>73.693693693693689</v>
+        <v>72.612612612612608</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>73.333333333333329</v>
+        <v>71.531531531531527</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>75.675675675675677</v>
+        <v>73.513513513513516</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>69.729729729729726</v>
+        <v>68.468468468468473</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>72.612612612612608</v>
+        <v>70.990990990990994</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>72.612612612612608</v>
+        <v>70.810810810810807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>80.36036036036036</v>
+        <v>78.918918918918919</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>81.081081081081081</v>
+        <v>79.099099099099107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>79.459459459459453</v>
+        <v>78.198198198198199</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>80.36036036036036</v>
+        <v>79.63963963963964</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>67.567567567567565</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>72.252252252252248</v>
+        <v>70.450450450450447</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76.21621621621621</v>
+        <v>75.855855855855864</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>76.396396396396398</v>
+        <v>75.13513513513513</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>76.936936936936945</v>
+        <v>75.13513513513513</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>64.324324324324323</v>
+        <v>63.243243243243242</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>67.567567567567565</v>
+        <v>66.486486486486484</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>71.171171171171167</v>
+        <v>70.090090090090087</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>77.837837837837839</v>
+        <v>76.576576576576571</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>79.099099099099107</v>
+        <v>78.198198198198199</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>78.378378378378372</v>
+        <v>76.936936936936945</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>66.486486486486484</v>
+        <v>65.765765765765778</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>64.324324324324323</v>
+        <v>63.063063063063062</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>64.14414414414415</v>
+        <v>62.702702702702709</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>75.49549549549549</v>
+        <v>73.873873873873876</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>71.891891891891888</v>
+        <v>70.270270270270274</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>74.054054054054049</v>
+        <v>70.990990990990994</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>72.792792792792795</v>
+        <v>70.990990990990994</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>69.549549549549553</v>
+        <v>67.747747747747738</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>72.972972972972968</v>
+        <v>70.630630630630634</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>75.315315315315317</v>
+        <v>72.612612612612608</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>75.855855855855864</v>
+        <v>73.693693693693689</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>76.036036036036037</v>
+        <v>73.873873873873876</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>69.009009009009006</v>
+        <v>67.567567567567565</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>69.549549549549553</v>
+        <v>68.108108108108112</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>62.882882882882882</v>
+        <v>61.981981981981981</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>70.990990990990994</v>
+        <v>69.369369369369366</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>66.306306306306311</v>
+        <v>64.684684684684697</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>66.666666666666657</v>
+        <v>65.765765765765778</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74.414414414414409</v>
+        <v>71.891891891891888</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>76.21621621621621</v>
+        <v>74.414414414414409</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>76.756756756756758</v>
+        <v>74.234234234234236</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>75.49549549549549</v>
+        <v>74.054054054054049</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>75.855855855855864</v>
+        <v>74.054054054054049</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>75.675675675675677</v>
+        <v>74.954954954954957</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>68.468468468468473</v>
+        <v>67.387387387387392</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>68.288288288288285</v>
+        <v>67.747747747747738</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>73.513513513513516</v>
+        <v>71.351351351351354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done to calculate the mean in all threhsolding algorithms
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -249,7 +267,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Solved the plot problem
</commit_message>
<xml_diff>
--- a/Thresholding/LocalT2/HK_G_acc_LT.xlsx
+++ b/Thresholding/LocalT2/HK_G_acc_LT.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
   <si>
     <t>HK_G_acc_LT</t>
   </si>
@@ -267,7 +270,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">

</xml_diff>